<commit_message>
for loop and working with string updated
</commit_message>
<xml_diff>
--- a/working on text and string data re and string functions.xlsx
+++ b/working on text and string data re and string functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\END_TO_END_PYTHON_PROJECT_YOUTUBE_SUPER_IMPORTANT\Python_End_To_End_Projects\Real Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC59D0-8F1E-48E1-8065-70B955B1A81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877215B5-2FDF-4AB2-A2AE-60DEC55E7E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73837C2D-3AF6-4B9F-ADD0-DEFB537B3163}"/>
   </bookViews>
@@ -777,145 +777,6 @@
 &gt;&gt;&gt; re_obj.search(s4)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">write r'before any pattern while using re
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.(dot)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	Matches any single character except newline,      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	Matches zero or more repetitions,    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> +</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	Matches one or more repetitions,   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	∙ Matches zero or one repetition,   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{}</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	Matches an explicitly specified number of repetitions,   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="48"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	Specifies a character class
-</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;&gt;&gt; m = re.search(r'(\w+),(\w+),(\w+)', 'foo,bar,baz')
 &gt;&gt;&gt; m.group(1, 3)
 ('foo', 'baz')
@@ -952,6 +813,144 @@
 '123bar456'
 &gt;&gt;&gt; m.span()
 (3, 12)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">write r'before any pattern while using re
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.(dot)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	Matches any single character except newline,      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	Matches zero or more repetitions,    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> +</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	Matches one or more repetitions,   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	∙ Matches zero or one repetition,   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	Matches an explicitly specified number of repetitions,   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	Specifies a character class</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1206,18 +1205,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1230,11 +1217,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1555,8 +1554,8 @@
   </sheetPr>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1565,7 +1564,7 @@
     <col min="2" max="2" width="71.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="70.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="76.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="188.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="45" style="1" customWidth="1"/>
     <col min="8" max="8" width="23.21875" style="1" customWidth="1"/>
@@ -1589,9 +1588,9 @@
       <c r="F1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="314.39999999999998" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -1608,9 +1607,9 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="201.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
@@ -1625,9 +1624,9 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:9" ht="228" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
@@ -1648,9 +1647,9 @@
       <c r="F4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9" ht="230.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
@@ -1669,9 +1668,9 @@
       <c r="F5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" ht="208.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
@@ -1688,9 +1687,9 @@
       <c r="F6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" ht="93.6" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
@@ -1703,9 +1702,9 @@
         <v>72</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" ht="283.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
@@ -1724,9 +1723,9 @@
       <c r="F8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" ht="230.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
@@ -1743,9 +1742,9 @@
       <c r="F9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" ht="338.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
@@ -1764,9 +1763,9 @@
       <c r="F10" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" ht="211.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
@@ -1783,9 +1782,9 @@
       <c r="F11" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" ht="232.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
@@ -1800,90 +1799,90 @@
       <c r="F12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" s="8" customFormat="1" ht="46.2" x14ac:dyDescent="0.7">
-      <c r="A13" s="21" t="s">
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" s="8" customFormat="1" ht="192.6" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" s="18" customFormat="1" ht="61.2" x14ac:dyDescent="1.1000000000000001">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" s="18" customFormat="1" ht="61.2" x14ac:dyDescent="1.1000000000000001">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" ht="61.2" x14ac:dyDescent="1.1000000000000001">
-      <c r="A16" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" s="24" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" s="18" customFormat="1" ht="262.8" customHeight="1" x14ac:dyDescent="1.1000000000000001">
+      <c r="A16" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="1:11" s="20" customFormat="1" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1891,7 +1890,7 @@
       <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="21" t="s">
         <v>106</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -1914,7 +1913,7 @@
     </row>
     <row r="19" spans="1:11" s="7" customFormat="1" ht="336" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="5"/>
-      <c r="B19" s="25"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="15"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
@@ -1988,7 +1987,7 @@
         <v>48</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -2001,7 +2000,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
@@ -2060,7 +2059,7 @@
         <v>48</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -2073,7 +2072,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
@@ -2102,7 +2101,7 @@
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:11" s="7" customFormat="1" ht="187.2" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:11" s="7" customFormat="1" ht="256.8" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="16" t="s">
         <v>24</v>
       </c>
@@ -2193,9 +2192,9 @@
       <c r="F33" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>